<commit_message>
garden page and video carosals
</commit_message>
<xml_diff>
--- a/backend/db/QBGDigitalGuide_data.xlsx
+++ b/backend/db/QBGDigitalGuide_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Projects\tour\backend\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D2063BA-06EC-4C6F-AA16-E8C8819EB219}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{047CC9C7-FC48-4D14-A824-D179C413D3EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27260" yWindow="-114" windowWidth="27603" windowHeight="15027" activeTab="1" xr2:uid="{09D21884-479E-467C-BD18-06F6FCF93B5C}"/>
+    <workbookView xWindow="-114" yWindow="-114" windowWidth="27602" windowHeight="15027" activeTab="1" xr2:uid="{09D21884-479E-467C-BD18-06F6FCF93B5C}"/>
   </bookViews>
   <sheets>
     <sheet name="months" sheetId="1" r:id="rId1"/>
@@ -2694,8 +2694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{139DBBB9-8D14-4BCA-A890-FF4B11EE2F7A}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33:B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -3136,13 +3136,14 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.140625" customWidth="1"/>
-    <col min="2" max="3" width="42.7109375" customWidth="1"/>
+    <col min="2" max="2" width="42.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
     <col min="4" max="4" width="110.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>